<commit_message>
1. Atualização dos tempos.
</commit_message>
<xml_diff>
--- a/instancias/resultados.xlsx
+++ b/instancias/resultados.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="25">
   <si>
     <t xml:space="preserve">Receptor</t>
   </si>
@@ -37,31 +37,61 @@
     <t xml:space="preserve">Corrompidos</t>
   </si>
   <si>
+    <t xml:space="preserve">Tempo</t>
+  </si>
+  <si>
     <t xml:space="preserve">t1</t>
   </si>
   <si>
+    <t xml:space="preserve">0m3,663s</t>
+  </si>
+  <si>
     <t xml:space="preserve">t2</t>
   </si>
   <si>
+    <t xml:space="preserve">0m3,240s</t>
+  </si>
+  <si>
     <t xml:space="preserve">t3</t>
   </si>
   <si>
+    <t xml:space="preserve">0m4,715s</t>
+  </si>
+  <si>
     <t xml:space="preserve">t4</t>
   </si>
   <si>
+    <t xml:space="preserve">0m3,879s</t>
+  </si>
+  <si>
     <t xml:space="preserve">t5</t>
   </si>
   <si>
+    <t xml:space="preserve">0m2,894s</t>
+  </si>
+  <si>
     <t xml:space="preserve">t6</t>
   </si>
   <si>
+    <t xml:space="preserve">0m4,589s</t>
+  </si>
+  <si>
     <t xml:space="preserve">t7</t>
   </si>
   <si>
+    <t xml:space="preserve">0m9,516s</t>
+  </si>
+  <si>
     <t xml:space="preserve">t8</t>
   </si>
   <si>
+    <t xml:space="preserve">0m3,633s</t>
+  </si>
+  <si>
     <t xml:space="preserve">t9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0m24,769s</t>
   </si>
   <si>
     <t xml:space="preserve">Remetente</t>
@@ -79,6 +109,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -99,6 +130,7 @@
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -148,7 +180,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -173,10 +205,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:M24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
+      <selection pane="topLeft" activeCell="G6" activeCellId="0" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -185,9 +217,11 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.03"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="17.22"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="17.21"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="7" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="15.69"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -198,6 +232,13 @@
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
+      <c r="I1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2"/>
@@ -213,171 +254,337 @@
       <c r="E2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="2"/>
+      <c r="F2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="C3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D3" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E3" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F3" s="2"/>
+      <c r="I3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J3" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="K3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M3" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B4" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="C4" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="D4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J4" s="2" t="n">
         <v>14</v>
       </c>
-      <c r="C4" s="2" t="n">
+      <c r="K4" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="D4" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E4" s="2" t="n">
+      <c r="L4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M4" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="F4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B5" s="2" t="n">
+        <v>26</v>
+      </c>
+      <c r="C5" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="D5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="2" t="n">
+        <v>17</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J5" s="2" t="n">
         <v>33</v>
       </c>
-      <c r="C5" s="2" t="n">
+      <c r="K5" s="2" t="n">
         <v>26</v>
       </c>
-      <c r="D5" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E5" s="2" t="n">
+      <c r="L5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M5" s="2" t="n">
         <v>19</v>
       </c>
-      <c r="F5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B6" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="C6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J6" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="C6" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D6" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E6" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F6" s="2"/>
+      <c r="K6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M6" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B7" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="C7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J7" s="2" t="n">
         <v>16</v>
       </c>
-      <c r="C7" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D7" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E7" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F7" s="2"/>
+      <c r="K7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M7" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B8" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="C8" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="D8" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="E8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J8" s="2" t="n">
         <v>15</v>
       </c>
-      <c r="C8" s="2" t="n">
+      <c r="K8" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="D8" s="2" t="n">
+      <c r="L8" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="E8" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F8" s="2"/>
+      <c r="M8" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="B9" s="2" t="n">
+        <v>28</v>
+      </c>
+      <c r="C9" s="2" t="n">
+        <v>17</v>
+      </c>
+      <c r="D9" s="2" t="n">
+        <v>17</v>
+      </c>
+      <c r="E9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J9" s="2" t="n">
         <v>41</v>
       </c>
-      <c r="C9" s="2" t="n">
+      <c r="K9" s="2" t="n">
         <v>27</v>
       </c>
-      <c r="D9" s="2" t="n">
+      <c r="L9" s="2" t="n">
         <v>27</v>
       </c>
-      <c r="E9" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F9" s="2"/>
+      <c r="M9" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="B10" s="2" t="n">
+        <v>29</v>
+      </c>
+      <c r="C10" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="D10" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="E10" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J10" s="2" t="n">
         <v>22</v>
       </c>
-      <c r="C10" s="2" t="n">
+      <c r="K10" s="2" t="n">
         <v>15</v>
       </c>
-      <c r="D10" s="2" t="n">
+      <c r="L10" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="E10" s="2" t="n">
+      <c r="M10" s="2" t="n">
         <v>9</v>
       </c>
-      <c r="F10" s="2"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="B11" s="2" t="n">
+        <v>91</v>
+      </c>
+      <c r="C11" s="2" t="n">
+        <v>76</v>
+      </c>
+      <c r="D11" s="2" t="n">
+        <v>51</v>
+      </c>
+      <c r="E11" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J11" s="2" t="n">
         <v>97</v>
       </c>
-      <c r="C11" s="2" t="n">
+      <c r="K11" s="2" t="n">
         <v>90</v>
       </c>
-      <c r="D11" s="2" t="n">
+      <c r="L11" s="2" t="n">
         <v>68</v>
       </c>
-      <c r="E11" s="2" t="n">
+      <c r="M11" s="2" t="n">
         <v>21</v>
       </c>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2"/>
@@ -386,18 +593,28 @@
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
+      <c r="I13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2"/>
@@ -413,37 +630,67 @@
       <c r="E14" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
+      <c r="F14" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="L14" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="M14" s="2" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B15" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="C15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J15" s="2" t="n">
         <v>9</v>
       </c>
-      <c r="C15" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D15" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E15" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
+      <c r="K15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M15" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B16" s="2" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C16" s="2" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D16" s="2" t="n">
         <v>0</v>
@@ -451,141 +698,269 @@
       <c r="E16" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
+      <c r="F16" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J16" s="2" t="n">
+        <v>17</v>
+      </c>
+      <c r="K16" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="L16" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M16" s="2" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B17" s="2" t="n">
+        <v>26</v>
+      </c>
+      <c r="C17" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="D17" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E17" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J17" s="2" t="n">
         <v>34</v>
       </c>
-      <c r="C17" s="2" t="n">
+      <c r="K17" s="2" t="n">
         <v>26</v>
       </c>
-      <c r="D17" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E17" s="2" t="n">
+      <c r="L17" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M17" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="B18" s="2" t="n">
+      <c r="C18" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D18" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E18" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J18" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="C18" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D18" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E18" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
+      <c r="K18" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L18" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M18" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="2" t="n">
         <v>9</v>
       </c>
-      <c r="B19" s="2" t="n">
+      <c r="C19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J19" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="C19" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D19" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E19" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
+      <c r="K19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M19" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B20" s="2" t="n">
+        <v>28</v>
+      </c>
+      <c r="C20" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="D20" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="E20" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J20" s="2" t="n">
         <v>19</v>
       </c>
-      <c r="C20" s="2" t="n">
+      <c r="K20" s="2" t="n">
         <v>11</v>
       </c>
-      <c r="D20" s="2" t="n">
+      <c r="L20" s="2" t="n">
         <v>9</v>
       </c>
-      <c r="E20" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
+      <c r="M20" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="B21" s="2" t="n">
+        <v>80</v>
+      </c>
+      <c r="C21" s="2" t="n">
+        <v>72</v>
+      </c>
+      <c r="D21" s="2" t="n">
+        <v>55</v>
+      </c>
+      <c r="E21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J21" s="2" t="n">
         <v>110</v>
       </c>
-      <c r="C21" s="2" t="n">
+      <c r="K21" s="2" t="n">
         <v>102</v>
       </c>
-      <c r="D21" s="2" t="n">
+      <c r="L21" s="2" t="n">
         <v>75</v>
       </c>
-      <c r="E21" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
+      <c r="M21" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="B22" s="2" t="n">
+        <v>33</v>
+      </c>
+      <c r="C22" s="2" t="n">
+        <v>25</v>
+      </c>
+      <c r="D22" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="E22" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J22" s="2" t="n">
         <v>31</v>
       </c>
-      <c r="C22" s="2" t="n">
+      <c r="K22" s="2" t="n">
         <v>21</v>
       </c>
-      <c r="D22" s="2" t="n">
+      <c r="L22" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="E22" s="2" t="n">
+      <c r="M22" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="B23" s="2" t="n">
+        <v>256</v>
+      </c>
+      <c r="C23" s="2" t="n">
+        <v>248</v>
+      </c>
+      <c r="D23" s="2" t="n">
+        <v>172</v>
+      </c>
+      <c r="E23" s="2" t="n">
+        <v>63</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J23" s="2" t="n">
         <v>309</v>
       </c>
-      <c r="C23" s="2" t="n">
+      <c r="K23" s="2" t="n">
         <v>297</v>
       </c>
-      <c r="D23" s="2" t="n">
+      <c r="L23" s="2" t="n">
         <v>207</v>
       </c>
-      <c r="E23" s="2" t="n">
+      <c r="M23" s="2" t="n">
         <v>66</v>
       </c>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -598,9 +973,11 @@
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="A1:E1"/>
+    <mergeCell ref="I1:M1"/>
     <mergeCell ref="A13:E13"/>
+    <mergeCell ref="I13:M13"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>